<commit_message>
Last version before add more things
</commit_message>
<xml_diff>
--- a/datos/datos_recalificar_todo.xlsx
+++ b/datos/datos_recalificar_todo.xlsx
@@ -5,11 +5,10 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="CURSOS" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="PREGUNTAS" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,18 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t xml:space="preserve">CURSOS_ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PREGUNTAS_ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T01.04.18,C003,N2[Movimiento rectilíneo uniforme]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">T02.03.34,B001,N1[Clases de fuerzas]</t>
   </si>
 </sst>
 </file>
@@ -130,7 +120,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -148,18 +138,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -182,8 +160,8 @@
   </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -210,7 +188,9 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3"/>
+      <c r="A4" s="3" t="n">
+        <v>12307</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3"/>
@@ -228,58 +208,4 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="51.55"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="5" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="3"/>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7"/>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3"/>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0"/>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>